<commit_message>
sizes fix and update
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="1090">
   <si>
     <t>Alone In The Dark 2</t>
   </si>
@@ -2824,6 +2824,471 @@
   </si>
   <si>
     <t>Yan's Dojo</t>
+  </si>
+  <si>
+    <t>Monkey Island 2</t>
+  </si>
+  <si>
+    <t>324533-monkey-island-2-lechuck-s-revenge-dos-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>Opening Themes &amp; Introduction</t>
+  </si>
+  <si>
+    <t>Phatt Island Map</t>
+  </si>
+  <si>
+    <t>Chapter Screen</t>
+  </si>
+  <si>
+    <t>Phatt Island Wheel Of Fortune</t>
+  </si>
+  <si>
+    <t>If This Is Three</t>
+  </si>
+  <si>
+    <t>Scabb Island Overview</t>
+  </si>
+  <si>
+    <t>Phatt Island Alley Dealer</t>
+  </si>
+  <si>
+    <t>Woodtick</t>
+  </si>
+  <si>
+    <t>Largo LaGrande</t>
+  </si>
+  <si>
+    <t>The Booty Boutique</t>
+  </si>
+  <si>
+    <t>Governor Marleys Guard House</t>
+  </si>
+  <si>
+    <t>The Swamp</t>
+  </si>
+  <si>
+    <t>Governor Marleys Mardi Gras Fish Fry</t>
+  </si>
+  <si>
+    <t>The Cemetery</t>
+  </si>
+  <si>
+    <t>Elaine And Guybrush</t>
+  </si>
+  <si>
+    <t>Stabbing Largo And LeChuck Returns</t>
+  </si>
+  <si>
+    <t>Stealing Elaines Map</t>
+  </si>
+  <si>
+    <t>The Cook</t>
+  </si>
+  <si>
+    <t>Captain Dread</t>
+  </si>
+  <si>
+    <t>Wow, What a Dream &amp; The Bone Song</t>
+  </si>
+  <si>
+    <t>Captain Dread And The Map</t>
+  </si>
+  <si>
+    <t>Woodtick Revisited</t>
+  </si>
+  <si>
+    <t>LeChucks Lament</t>
+  </si>
+  <si>
+    <t>Phatt Island</t>
+  </si>
+  <si>
+    <t>Phatt Island Jail</t>
+  </si>
+  <si>
+    <t>Rooms Of Ugly Bone Things</t>
+  </si>
+  <si>
+    <t>Outside Phatt Mansion</t>
+  </si>
+  <si>
+    <t>The Escape From LeChucks Fortress</t>
+  </si>
+  <si>
+    <t>Phatt Mansion Guard</t>
+  </si>
+  <si>
+    <t>The Voodoo Dolly</t>
+  </si>
+  <si>
+    <t>Governeur Phatts Room</t>
+  </si>
+  <si>
+    <t>The Underground Tunnels</t>
+  </si>
+  <si>
+    <t>Closing Themes</t>
+  </si>
+  <si>
+    <t>Stans Previously Used Coffins</t>
+  </si>
+  <si>
+    <t>Monkey Island 2 - Medley (Bonus)</t>
+  </si>
+  <si>
+    <t>The Crypt - Rapp Scallion</t>
+  </si>
+  <si>
+    <t>The Spitting Contest</t>
+  </si>
+  <si>
+    <t>Captain Kates Boat - Booty Island</t>
+  </si>
+  <si>
+    <t>Jojo The Monkey</t>
+  </si>
+  <si>
+    <t>Phatt Island Waterfall</t>
+  </si>
+  <si>
+    <t>Secret Waterfall Tunnel</t>
+  </si>
+  <si>
+    <t>Rum Rogers Cottage Exteriors</t>
+  </si>
+  <si>
+    <t>The Drinking Contest</t>
+  </si>
+  <si>
+    <t>Return of Largo LaGrande (Bonus)</t>
+  </si>
+  <si>
+    <t>Underground Club</t>
+  </si>
+  <si>
+    <t>Fight in Underground Club</t>
+  </si>
+  <si>
+    <t>New Arbat Club</t>
+  </si>
+  <si>
+    <t>Kick from New Arbat</t>
+  </si>
+  <si>
+    <t>Mutant Club</t>
+  </si>
+  <si>
+    <t>Kick from Mutant Club</t>
+  </si>
+  <si>
+    <t>Titan Club</t>
+  </si>
+  <si>
+    <t>Kick from Titan Club</t>
+  </si>
+  <si>
+    <t>Butterfly Club</t>
+  </si>
+  <si>
+    <t>With Girl from Butterfly Club</t>
+  </si>
+  <si>
+    <t>Gold Kozel Club</t>
+  </si>
+  <si>
+    <t>The Provincial Player</t>
+  </si>
+  <si>
+    <t>2017-11-06-17-50-43-3861.jpg</t>
+  </si>
+  <si>
+    <t>Command &amp; Conquer: Red Alert</t>
+  </si>
+  <si>
+    <t>Hell March</t>
+  </si>
+  <si>
+    <t>Workmen</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Twin Cannon</t>
+  </si>
+  <si>
+    <t>Terminate</t>
+  </si>
+  <si>
+    <t>Smash</t>
+  </si>
+  <si>
+    <t>Roll Out</t>
+  </si>
+  <si>
+    <t>Radio 2</t>
+  </si>
+  <si>
+    <t>Mud</t>
+  </si>
+  <si>
+    <t>Militant Force (Score Theme)</t>
+  </si>
+  <si>
+    <t>Fogger</t>
+  </si>
+  <si>
+    <t>Face the Enemy</t>
+  </si>
+  <si>
+    <t>Dense</t>
+  </si>
+  <si>
+    <t>Crush</t>
+  </si>
+  <si>
+    <t>Big Foot</t>
+  </si>
+  <si>
+    <t>Trenches</t>
+  </si>
+  <si>
+    <t>Face the Enemy 1</t>
+  </si>
+  <si>
+    <t>81033-command-conquer-red-alert-dos-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>Voice Rhythm 2</t>
+  </si>
+  <si>
+    <t>Underlying Thoughts</t>
+  </si>
+  <si>
+    <t>The Second Hand</t>
+  </si>
+  <si>
+    <t>Shut It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radio 2 Remix </t>
+  </si>
+  <si>
+    <t>Journey</t>
+  </si>
+  <si>
+    <t>Chaos</t>
+  </si>
+  <si>
+    <t>Backstab</t>
+  </si>
+  <si>
+    <t>Arazoid</t>
+  </si>
+  <si>
+    <t>Command &amp; Conquer: Red Alert – Counterstrike</t>
+  </si>
+  <si>
+    <t>27424-command-conquer-red-alert-counterstrike-dos-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>Command &amp; Conquer: Red Alert – The Aftermath</t>
+  </si>
+  <si>
+    <t>Wasteland</t>
+  </si>
+  <si>
+    <t>Traction</t>
+  </si>
+  <si>
+    <t>The Search</t>
+  </si>
+  <si>
+    <t>Running through pipes</t>
+  </si>
+  <si>
+    <t>Groundwire</t>
+  </si>
+  <si>
+    <t>Floating</t>
+  </si>
+  <si>
+    <t>Bog</t>
+  </si>
+  <si>
+    <t>26999-command-conquer-red-alert-the-aftermath-dos-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>Sam &amp; Max Hit the Road</t>
+  </si>
+  <si>
+    <t>''Friends...'' (Complete)</t>
+  </si>
+  <si>
+    <t>Pleasently Understated Credit Sequence</t>
+  </si>
+  <si>
+    <t>Another Idiotic and Baffling Assignment</t>
+  </si>
+  <si>
+    <t>Outside Headquarters</t>
+  </si>
+  <si>
+    <t>Carnival of the Odd</t>
+  </si>
+  <si>
+    <t>Wak-a-Rat</t>
+  </si>
+  <si>
+    <t>Hall of Oddities</t>
+  </si>
+  <si>
+    <t>Trixie's Trailer</t>
+  </si>
+  <si>
+    <t>Doug the Moleman</t>
+  </si>
+  <si>
+    <t>Greetings from the USA</t>
+  </si>
+  <si>
+    <t>Highway Surfing</t>
+  </si>
+  <si>
+    <t>The World's Largest Ball of Twine</t>
+  </si>
+  <si>
+    <t>World of Fish &amp; ''I'm a Trout, Stupid''</t>
+  </si>
+  <si>
+    <t>Dino Bungee National Memorial</t>
+  </si>
+  <si>
+    <t>Extracting the Tooth from a Per... Predator</t>
+  </si>
+  <si>
+    <t>Celebrity Vegetable Museum</t>
+  </si>
+  <si>
+    <t>Childhood in Brighton</t>
+  </si>
+  <si>
+    <t>Virtual Reality or The Tale of Brave Sir Sam</t>
+  </si>
+  <si>
+    <t>Savage Jungle Inn</t>
+  </si>
+  <si>
+    <t>Bigfoot Party</t>
+  </si>
+  <si>
+    <t>End Titles</t>
+  </si>
+  <si>
+    <t>Highway</t>
+  </si>
+  <si>
+    <t>249177-sam-max-hit-the-road-dos-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>69781-killing-time-windows-front-cover.jpg</t>
+  </si>
+  <si>
+    <t>Killing Time</t>
+  </si>
+  <si>
+    <t>Track 11</t>
+  </si>
+  <si>
+    <t>Track 12</t>
+  </si>
+  <si>
+    <t>Track 14</t>
+  </si>
+  <si>
+    <t>Track 16</t>
+  </si>
+  <si>
+    <t>Track 17</t>
+  </si>
+  <si>
+    <t>Track 18</t>
+  </si>
+  <si>
+    <t>Track 19</t>
+  </si>
+  <si>
+    <t>Track 20</t>
+  </si>
+  <si>
+    <t>Track 21</t>
+  </si>
+  <si>
+    <t>Track 22</t>
+  </si>
+  <si>
+    <t>Track 23</t>
+  </si>
+  <si>
+    <t>Track 24</t>
+  </si>
+  <si>
+    <t>Track 25</t>
+  </si>
+  <si>
+    <t>Track 26</t>
+  </si>
+  <si>
+    <t>Track 27</t>
+  </si>
+  <si>
+    <t>Track 28</t>
+  </si>
+  <si>
+    <t>Track 29</t>
+  </si>
+  <si>
+    <t>Track 30</t>
+  </si>
+  <si>
+    <t>Track 31</t>
+  </si>
+  <si>
+    <t>Track 32</t>
+  </si>
+  <si>
+    <t>Track 33</t>
+  </si>
+  <si>
+    <t>Track 34</t>
+  </si>
+  <si>
+    <t>Track 35</t>
+  </si>
+  <si>
+    <t>Track 36</t>
+  </si>
+  <si>
+    <t>Track 37</t>
+  </si>
+  <si>
+    <t>Track 38</t>
+  </si>
+  <si>
+    <t>Track 39</t>
+  </si>
+  <si>
+    <t>Track 40</t>
+  </si>
+  <si>
+    <t>Track 41</t>
+  </si>
+  <si>
+    <t>Track 42</t>
+  </si>
+  <si>
+    <t>Track 43</t>
   </si>
 </sst>
 </file>
@@ -3183,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J876"/>
+  <dimension ref="A2:J1035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A844" workbookViewId="0">
-      <selection activeCell="B869" sqref="B869"/>
+    <sheetView tabSelected="1" topLeftCell="A981" workbookViewId="0">
+      <selection activeCell="I1018" sqref="I1018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17900,6 +18365,2709 @@
         <v>910</v>
       </c>
     </row>
+    <row r="877" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A877">
+        <v>876</v>
+      </c>
+      <c r="B877" t="s">
+        <v>937</v>
+      </c>
+      <c r="C877" t="s">
+        <v>935</v>
+      </c>
+      <c r="D877">
+        <v>1991</v>
+      </c>
+      <c r="E877" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A878">
+        <v>877</v>
+      </c>
+      <c r="B878" t="s">
+        <v>938</v>
+      </c>
+      <c r="C878" t="s">
+        <v>935</v>
+      </c>
+      <c r="D878">
+        <v>1991</v>
+      </c>
+      <c r="E878" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A879">
+        <v>878</v>
+      </c>
+      <c r="B879" t="s">
+        <v>939</v>
+      </c>
+      <c r="C879" t="s">
+        <v>935</v>
+      </c>
+      <c r="D879">
+        <v>1991</v>
+      </c>
+      <c r="E879" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A880">
+        <v>879</v>
+      </c>
+      <c r="B880" t="s">
+        <v>940</v>
+      </c>
+      <c r="C880" t="s">
+        <v>935</v>
+      </c>
+      <c r="D880">
+        <v>1991</v>
+      </c>
+      <c r="E880" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A881">
+        <v>880</v>
+      </c>
+      <c r="B881" t="s">
+        <v>941</v>
+      </c>
+      <c r="C881" t="s">
+        <v>935</v>
+      </c>
+      <c r="D881">
+        <v>1991</v>
+      </c>
+      <c r="E881" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A882">
+        <v>881</v>
+      </c>
+      <c r="B882" t="s">
+        <v>942</v>
+      </c>
+      <c r="C882" t="s">
+        <v>935</v>
+      </c>
+      <c r="D882">
+        <v>1991</v>
+      </c>
+      <c r="E882" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A883">
+        <v>882</v>
+      </c>
+      <c r="B883" t="s">
+        <v>943</v>
+      </c>
+      <c r="C883" t="s">
+        <v>935</v>
+      </c>
+      <c r="D883">
+        <v>1991</v>
+      </c>
+      <c r="E883" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A884">
+        <v>883</v>
+      </c>
+      <c r="B884" t="s">
+        <v>944</v>
+      </c>
+      <c r="C884" t="s">
+        <v>935</v>
+      </c>
+      <c r="D884">
+        <v>1991</v>
+      </c>
+      <c r="E884" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A885">
+        <v>884</v>
+      </c>
+      <c r="B885" t="s">
+        <v>945</v>
+      </c>
+      <c r="C885" t="s">
+        <v>935</v>
+      </c>
+      <c r="D885">
+        <v>1991</v>
+      </c>
+      <c r="E885" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A886">
+        <v>885</v>
+      </c>
+      <c r="B886" t="s">
+        <v>946</v>
+      </c>
+      <c r="C886" t="s">
+        <v>935</v>
+      </c>
+      <c r="D886">
+        <v>1991</v>
+      </c>
+      <c r="E886" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A887">
+        <v>886</v>
+      </c>
+      <c r="B887" t="s">
+        <v>947</v>
+      </c>
+      <c r="C887" t="s">
+        <v>935</v>
+      </c>
+      <c r="D887">
+        <v>1991</v>
+      </c>
+      <c r="E887" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A888">
+        <v>887</v>
+      </c>
+      <c r="B888" t="s">
+        <v>948</v>
+      </c>
+      <c r="C888" t="s">
+        <v>935</v>
+      </c>
+      <c r="D888">
+        <v>1991</v>
+      </c>
+      <c r="E888" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A889">
+        <v>888</v>
+      </c>
+      <c r="B889" t="s">
+        <v>949</v>
+      </c>
+      <c r="C889" t="s">
+        <v>935</v>
+      </c>
+      <c r="D889">
+        <v>1991</v>
+      </c>
+      <c r="E889" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A890">
+        <v>889</v>
+      </c>
+      <c r="B890" t="s">
+        <v>950</v>
+      </c>
+      <c r="C890" t="s">
+        <v>935</v>
+      </c>
+      <c r="D890">
+        <v>1991</v>
+      </c>
+      <c r="E890" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="891" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A891">
+        <v>890</v>
+      </c>
+      <c r="B891" t="s">
+        <v>951</v>
+      </c>
+      <c r="C891" t="s">
+        <v>935</v>
+      </c>
+      <c r="D891">
+        <v>1991</v>
+      </c>
+      <c r="E891" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="892" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A892">
+        <v>891</v>
+      </c>
+      <c r="B892" t="s">
+        <v>952</v>
+      </c>
+      <c r="C892" t="s">
+        <v>935</v>
+      </c>
+      <c r="D892">
+        <v>1991</v>
+      </c>
+      <c r="E892" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="893" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A893">
+        <v>892</v>
+      </c>
+      <c r="B893" t="s">
+        <v>953</v>
+      </c>
+      <c r="C893" t="s">
+        <v>935</v>
+      </c>
+      <c r="D893">
+        <v>1991</v>
+      </c>
+      <c r="E893" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="894" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A894">
+        <v>893</v>
+      </c>
+      <c r="B894" t="s">
+        <v>954</v>
+      </c>
+      <c r="C894" t="s">
+        <v>935</v>
+      </c>
+      <c r="D894">
+        <v>1991</v>
+      </c>
+      <c r="E894" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A895">
+        <v>894</v>
+      </c>
+      <c r="B895" t="s">
+        <v>955</v>
+      </c>
+      <c r="C895" t="s">
+        <v>935</v>
+      </c>
+      <c r="D895">
+        <v>1991</v>
+      </c>
+      <c r="E895" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="896" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A896">
+        <v>895</v>
+      </c>
+      <c r="B896" t="s">
+        <v>956</v>
+      </c>
+      <c r="C896" t="s">
+        <v>935</v>
+      </c>
+      <c r="D896">
+        <v>1991</v>
+      </c>
+      <c r="E896" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="897" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A897">
+        <v>896</v>
+      </c>
+      <c r="B897" t="s">
+        <v>957</v>
+      </c>
+      <c r="C897" t="s">
+        <v>935</v>
+      </c>
+      <c r="D897">
+        <v>1991</v>
+      </c>
+      <c r="E897" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="898" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A898">
+        <v>897</v>
+      </c>
+      <c r="B898" t="s">
+        <v>958</v>
+      </c>
+      <c r="C898" t="s">
+        <v>935</v>
+      </c>
+      <c r="D898">
+        <v>1991</v>
+      </c>
+      <c r="E898" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="899" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A899">
+        <v>898</v>
+      </c>
+      <c r="B899" t="s">
+        <v>959</v>
+      </c>
+      <c r="C899" t="s">
+        <v>935</v>
+      </c>
+      <c r="D899">
+        <v>1991</v>
+      </c>
+      <c r="E899" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="900" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A900">
+        <v>899</v>
+      </c>
+      <c r="B900" t="s">
+        <v>960</v>
+      </c>
+      <c r="C900" t="s">
+        <v>935</v>
+      </c>
+      <c r="D900">
+        <v>1991</v>
+      </c>
+      <c r="E900" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="901" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A901">
+        <v>900</v>
+      </c>
+      <c r="B901" t="s">
+        <v>961</v>
+      </c>
+      <c r="C901" t="s">
+        <v>935</v>
+      </c>
+      <c r="D901">
+        <v>1991</v>
+      </c>
+      <c r="E901" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="902" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A902">
+        <v>901</v>
+      </c>
+      <c r="B902" t="s">
+        <v>962</v>
+      </c>
+      <c r="C902" t="s">
+        <v>935</v>
+      </c>
+      <c r="D902">
+        <v>1991</v>
+      </c>
+      <c r="E902" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="903" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A903">
+        <v>902</v>
+      </c>
+      <c r="B903" t="s">
+        <v>963</v>
+      </c>
+      <c r="C903" t="s">
+        <v>935</v>
+      </c>
+      <c r="D903">
+        <v>1991</v>
+      </c>
+      <c r="E903" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="904" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A904">
+        <v>903</v>
+      </c>
+      <c r="B904" t="s">
+        <v>964</v>
+      </c>
+      <c r="C904" t="s">
+        <v>935</v>
+      </c>
+      <c r="D904">
+        <v>1991</v>
+      </c>
+      <c r="E904" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="905" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A905">
+        <v>904</v>
+      </c>
+      <c r="B905" t="s">
+        <v>965</v>
+      </c>
+      <c r="C905" t="s">
+        <v>935</v>
+      </c>
+      <c r="D905">
+        <v>1991</v>
+      </c>
+      <c r="E905" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="906" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A906">
+        <v>905</v>
+      </c>
+      <c r="B906" t="s">
+        <v>966</v>
+      </c>
+      <c r="C906" t="s">
+        <v>935</v>
+      </c>
+      <c r="D906">
+        <v>1991</v>
+      </c>
+      <c r="E906" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="907" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A907">
+        <v>906</v>
+      </c>
+      <c r="B907" t="s">
+        <v>967</v>
+      </c>
+      <c r="C907" t="s">
+        <v>935</v>
+      </c>
+      <c r="D907">
+        <v>1991</v>
+      </c>
+      <c r="E907" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="908" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A908">
+        <v>907</v>
+      </c>
+      <c r="B908" t="s">
+        <v>968</v>
+      </c>
+      <c r="C908" t="s">
+        <v>935</v>
+      </c>
+      <c r="D908">
+        <v>1991</v>
+      </c>
+      <c r="E908" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="909" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A909">
+        <v>908</v>
+      </c>
+      <c r="B909" t="s">
+        <v>969</v>
+      </c>
+      <c r="C909" t="s">
+        <v>935</v>
+      </c>
+      <c r="D909">
+        <v>1991</v>
+      </c>
+      <c r="E909" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="910" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A910">
+        <v>909</v>
+      </c>
+      <c r="B910" t="s">
+        <v>970</v>
+      </c>
+      <c r="C910" t="s">
+        <v>935</v>
+      </c>
+      <c r="D910">
+        <v>1991</v>
+      </c>
+      <c r="E910" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="911" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A911">
+        <v>910</v>
+      </c>
+      <c r="B911" t="s">
+        <v>971</v>
+      </c>
+      <c r="C911" t="s">
+        <v>935</v>
+      </c>
+      <c r="D911">
+        <v>1991</v>
+      </c>
+      <c r="E911" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="912" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A912">
+        <v>911</v>
+      </c>
+      <c r="B912" t="s">
+        <v>972</v>
+      </c>
+      <c r="C912" t="s">
+        <v>935</v>
+      </c>
+      <c r="D912">
+        <v>1991</v>
+      </c>
+      <c r="E912" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="913" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A913">
+        <v>912</v>
+      </c>
+      <c r="B913" t="s">
+        <v>973</v>
+      </c>
+      <c r="C913" t="s">
+        <v>935</v>
+      </c>
+      <c r="D913">
+        <v>1991</v>
+      </c>
+      <c r="E913" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="914" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A914">
+        <v>913</v>
+      </c>
+      <c r="B914" t="s">
+        <v>974</v>
+      </c>
+      <c r="C914" t="s">
+        <v>935</v>
+      </c>
+      <c r="D914">
+        <v>1991</v>
+      </c>
+      <c r="E914" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="915" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A915">
+        <v>914</v>
+      </c>
+      <c r="B915" t="s">
+        <v>975</v>
+      </c>
+      <c r="C915" t="s">
+        <v>935</v>
+      </c>
+      <c r="D915">
+        <v>1991</v>
+      </c>
+      <c r="E915" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="916" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A916">
+        <v>915</v>
+      </c>
+      <c r="B916" t="s">
+        <v>976</v>
+      </c>
+      <c r="C916" t="s">
+        <v>935</v>
+      </c>
+      <c r="D916">
+        <v>1991</v>
+      </c>
+      <c r="E916" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="917" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A917">
+        <v>916</v>
+      </c>
+      <c r="B917" t="s">
+        <v>977</v>
+      </c>
+      <c r="C917" t="s">
+        <v>935</v>
+      </c>
+      <c r="D917">
+        <v>1991</v>
+      </c>
+      <c r="E917" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A918">
+        <v>917</v>
+      </c>
+      <c r="B918" t="s">
+        <v>978</v>
+      </c>
+      <c r="C918" t="s">
+        <v>935</v>
+      </c>
+      <c r="D918">
+        <v>1991</v>
+      </c>
+      <c r="E918" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="919" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A919">
+        <v>918</v>
+      </c>
+      <c r="B919" t="s">
+        <v>979</v>
+      </c>
+      <c r="C919" t="s">
+        <v>935</v>
+      </c>
+      <c r="D919">
+        <v>1991</v>
+      </c>
+      <c r="E919" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="920" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A920">
+        <v>919</v>
+      </c>
+      <c r="B920" t="s">
+        <v>980</v>
+      </c>
+      <c r="C920" t="s">
+        <v>935</v>
+      </c>
+      <c r="D920">
+        <v>1991</v>
+      </c>
+      <c r="E920" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="921" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A921">
+        <v>920</v>
+      </c>
+      <c r="B921" t="s">
+        <v>72</v>
+      </c>
+      <c r="C921" t="s">
+        <v>935</v>
+      </c>
+      <c r="D921">
+        <v>1991</v>
+      </c>
+      <c r="E921" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="922" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A922">
+        <v>921</v>
+      </c>
+      <c r="B922" t="s">
+        <v>3</v>
+      </c>
+      <c r="C922" t="s">
+        <v>992</v>
+      </c>
+      <c r="D922">
+        <v>1997</v>
+      </c>
+      <c r="E922" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="923" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A923">
+        <v>922</v>
+      </c>
+      <c r="B923" t="s">
+        <v>8</v>
+      </c>
+      <c r="C923" t="s">
+        <v>992</v>
+      </c>
+      <c r="D923">
+        <v>1997</v>
+      </c>
+      <c r="E923" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="924" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A924">
+        <v>923</v>
+      </c>
+      <c r="B924" t="s">
+        <v>981</v>
+      </c>
+      <c r="C924" t="s">
+        <v>992</v>
+      </c>
+      <c r="D924">
+        <v>1997</v>
+      </c>
+      <c r="E924" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="925" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A925">
+        <v>924</v>
+      </c>
+      <c r="B925" t="s">
+        <v>982</v>
+      </c>
+      <c r="C925" t="s">
+        <v>992</v>
+      </c>
+      <c r="D925">
+        <v>1997</v>
+      </c>
+      <c r="E925" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="926" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A926">
+        <v>925</v>
+      </c>
+      <c r="B926" t="s">
+        <v>983</v>
+      </c>
+      <c r="C926" t="s">
+        <v>992</v>
+      </c>
+      <c r="D926">
+        <v>1997</v>
+      </c>
+      <c r="E926" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="927" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A927">
+        <v>926</v>
+      </c>
+      <c r="B927" t="s">
+        <v>984</v>
+      </c>
+      <c r="C927" t="s">
+        <v>992</v>
+      </c>
+      <c r="D927">
+        <v>1997</v>
+      </c>
+      <c r="E927" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="928" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A928">
+        <v>927</v>
+      </c>
+      <c r="B928" t="s">
+        <v>985</v>
+      </c>
+      <c r="C928" t="s">
+        <v>992</v>
+      </c>
+      <c r="D928">
+        <v>1997</v>
+      </c>
+      <c r="E928" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="929" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A929">
+        <v>928</v>
+      </c>
+      <c r="B929" t="s">
+        <v>986</v>
+      </c>
+      <c r="C929" t="s">
+        <v>992</v>
+      </c>
+      <c r="D929">
+        <v>1997</v>
+      </c>
+      <c r="E929" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="930" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A930">
+        <v>929</v>
+      </c>
+      <c r="B930" t="s">
+        <v>987</v>
+      </c>
+      <c r="C930" t="s">
+        <v>992</v>
+      </c>
+      <c r="D930">
+        <v>1997</v>
+      </c>
+      <c r="E930" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="931" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A931">
+        <v>930</v>
+      </c>
+      <c r="B931" t="s">
+        <v>988</v>
+      </c>
+      <c r="C931" t="s">
+        <v>992</v>
+      </c>
+      <c r="D931">
+        <v>1997</v>
+      </c>
+      <c r="E931" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="932" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A932">
+        <v>931</v>
+      </c>
+      <c r="B932" t="s">
+        <v>989</v>
+      </c>
+      <c r="C932" t="s">
+        <v>992</v>
+      </c>
+      <c r="D932">
+        <v>1997</v>
+      </c>
+      <c r="E932" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="933" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A933">
+        <v>932</v>
+      </c>
+      <c r="B933" t="s">
+        <v>990</v>
+      </c>
+      <c r="C933" t="s">
+        <v>992</v>
+      </c>
+      <c r="D933">
+        <v>1997</v>
+      </c>
+      <c r="E933" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="934" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A934">
+        <v>933</v>
+      </c>
+      <c r="B934" t="s">
+        <v>991</v>
+      </c>
+      <c r="C934" t="s">
+        <v>992</v>
+      </c>
+      <c r="D934">
+        <v>1997</v>
+      </c>
+      <c r="E934" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="935" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A935">
+        <v>934</v>
+      </c>
+      <c r="B935" t="s">
+        <v>995</v>
+      </c>
+      <c r="C935" t="s">
+        <v>994</v>
+      </c>
+      <c r="D935">
+        <v>1996</v>
+      </c>
+      <c r="E935" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="936" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A936">
+        <v>935</v>
+      </c>
+      <c r="B936" t="s">
+        <v>996</v>
+      </c>
+      <c r="C936" t="s">
+        <v>994</v>
+      </c>
+      <c r="D936">
+        <v>1996</v>
+      </c>
+      <c r="E936" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="937" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A937">
+        <v>936</v>
+      </c>
+      <c r="B937" t="s">
+        <v>997</v>
+      </c>
+      <c r="C937" t="s">
+        <v>994</v>
+      </c>
+      <c r="D937">
+        <v>1996</v>
+      </c>
+      <c r="E937" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="938" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A938">
+        <v>937</v>
+      </c>
+      <c r="B938" t="s">
+        <v>998</v>
+      </c>
+      <c r="C938" t="s">
+        <v>994</v>
+      </c>
+      <c r="D938">
+        <v>1996</v>
+      </c>
+      <c r="E938" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="939" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A939">
+        <v>938</v>
+      </c>
+      <c r="B939" t="s">
+        <v>999</v>
+      </c>
+      <c r="C939" t="s">
+        <v>994</v>
+      </c>
+      <c r="D939">
+        <v>1996</v>
+      </c>
+      <c r="E939" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="940" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A940">
+        <v>939</v>
+      </c>
+      <c r="B940" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C940" t="s">
+        <v>994</v>
+      </c>
+      <c r="D940">
+        <v>1996</v>
+      </c>
+      <c r="E940" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="941" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A941">
+        <v>940</v>
+      </c>
+      <c r="B941" t="s">
+        <v>746</v>
+      </c>
+      <c r="C941" t="s">
+        <v>994</v>
+      </c>
+      <c r="D941">
+        <v>1996</v>
+      </c>
+      <c r="E941" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="942" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A942">
+        <v>941</v>
+      </c>
+      <c r="B942" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C942" t="s">
+        <v>994</v>
+      </c>
+      <c r="D942">
+        <v>1996</v>
+      </c>
+      <c r="E942" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="943" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A943">
+        <v>942</v>
+      </c>
+      <c r="B943" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C943" t="s">
+        <v>994</v>
+      </c>
+      <c r="D943">
+        <v>1996</v>
+      </c>
+      <c r="E943" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="944" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A944">
+        <v>943</v>
+      </c>
+      <c r="B944" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C944" t="s">
+        <v>994</v>
+      </c>
+      <c r="D944">
+        <v>1996</v>
+      </c>
+      <c r="E944" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="945" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A945">
+        <v>944</v>
+      </c>
+      <c r="B945" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C945" t="s">
+        <v>994</v>
+      </c>
+      <c r="D945">
+        <v>1996</v>
+      </c>
+      <c r="E945" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="946" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A946">
+        <v>945</v>
+      </c>
+      <c r="B946" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C946" t="s">
+        <v>994</v>
+      </c>
+      <c r="D946">
+        <v>1996</v>
+      </c>
+      <c r="E946" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="947" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A947">
+        <v>946</v>
+      </c>
+      <c r="B947" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C947" t="s">
+        <v>994</v>
+      </c>
+      <c r="D947">
+        <v>1996</v>
+      </c>
+      <c r="E947" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="948" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A948">
+        <v>947</v>
+      </c>
+      <c r="B948" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C948" t="s">
+        <v>994</v>
+      </c>
+      <c r="D948">
+        <v>1996</v>
+      </c>
+      <c r="E948" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="949" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A949">
+        <v>948</v>
+      </c>
+      <c r="B949" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C949" t="s">
+        <v>994</v>
+      </c>
+      <c r="D949">
+        <v>1996</v>
+      </c>
+      <c r="E949" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="950" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A950">
+        <v>949</v>
+      </c>
+      <c r="B950" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C950" t="s">
+        <v>994</v>
+      </c>
+      <c r="D950">
+        <v>1996</v>
+      </c>
+      <c r="E950" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="951" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A951">
+        <v>950</v>
+      </c>
+      <c r="B951" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C951" t="s">
+        <v>994</v>
+      </c>
+      <c r="D951">
+        <v>1996</v>
+      </c>
+      <c r="E951" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="952" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A952">
+        <v>951</v>
+      </c>
+      <c r="B952" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C952" t="s">
+        <v>994</v>
+      </c>
+      <c r="D952">
+        <v>1996</v>
+      </c>
+      <c r="E952" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="953" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A953">
+        <v>952</v>
+      </c>
+      <c r="B953" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C953" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D953">
+        <v>1997</v>
+      </c>
+      <c r="E953" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="954" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A954">
+        <v>953</v>
+      </c>
+      <c r="B954" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C954" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D954">
+        <v>1997</v>
+      </c>
+      <c r="E954" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="955" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A955">
+        <v>954</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C955" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D955">
+        <v>1997</v>
+      </c>
+      <c r="E955" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="956" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A956">
+        <v>955</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C956" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D956">
+        <v>1997</v>
+      </c>
+      <c r="E956" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="957" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A957">
+        <v>956</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C957" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D957">
+        <v>1997</v>
+      </c>
+      <c r="E957" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="958" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A958">
+        <v>957</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C958" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D958">
+        <v>1997</v>
+      </c>
+      <c r="E958" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="959" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A959">
+        <v>958</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C959" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D959">
+        <v>1997</v>
+      </c>
+      <c r="E959" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="960" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A960">
+        <v>959</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C960" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D960">
+        <v>1997</v>
+      </c>
+      <c r="E960" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="961" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A961">
+        <v>960</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C961" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D961">
+        <v>1997</v>
+      </c>
+      <c r="E961" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="962" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A962">
+        <v>961</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C962" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D962">
+        <v>1997</v>
+      </c>
+      <c r="E962" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="963" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A963">
+        <v>962</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C963" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D963">
+        <v>1997</v>
+      </c>
+      <c r="E963" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="964" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A964">
+        <v>963</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C964" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D964">
+        <v>1997</v>
+      </c>
+      <c r="E964" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="965" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A965">
+        <v>964</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C965" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D965">
+        <v>1997</v>
+      </c>
+      <c r="E965" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="966" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A966">
+        <v>965</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C966" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D966">
+        <v>1997</v>
+      </c>
+      <c r="E966" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="967" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A967">
+        <v>966</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C967" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D967">
+        <v>1997</v>
+      </c>
+      <c r="E967" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="968" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A968">
+        <v>967</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C968" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D968">
+        <v>1997</v>
+      </c>
+      <c r="E968" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="969" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A969">
+        <v>968</v>
+      </c>
+      <c r="B969" t="s">
+        <v>393</v>
+      </c>
+      <c r="C969" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D969">
+        <v>1997</v>
+      </c>
+      <c r="E969" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="970" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A970">
+        <v>969</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C970" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D970">
+        <v>1993</v>
+      </c>
+      <c r="E970" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="971" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A971">
+        <v>970</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C971" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D971">
+        <v>1993</v>
+      </c>
+      <c r="E971" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="972" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A972">
+        <v>971</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C972" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D972">
+        <v>1993</v>
+      </c>
+      <c r="E972" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="973" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A973">
+        <v>972</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C973" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D973">
+        <v>1993</v>
+      </c>
+      <c r="E973" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="974" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A974">
+        <v>973</v>
+      </c>
+      <c r="B974" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C974" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D974">
+        <v>1993</v>
+      </c>
+      <c r="E974" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="975" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A975">
+        <v>974</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C975" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D975">
+        <v>1993</v>
+      </c>
+      <c r="E975" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="976" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A976">
+        <v>975</v>
+      </c>
+      <c r="B976" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C976" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D976">
+        <v>1993</v>
+      </c>
+      <c r="E976" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="977" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A977">
+        <v>976</v>
+      </c>
+      <c r="B977" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C977" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D977">
+        <v>1993</v>
+      </c>
+      <c r="E977" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="978" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A978">
+        <v>977</v>
+      </c>
+      <c r="B978" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C978" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D978">
+        <v>1993</v>
+      </c>
+      <c r="E978" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="979" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A979">
+        <v>978</v>
+      </c>
+      <c r="B979" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C979" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D979">
+        <v>1993</v>
+      </c>
+      <c r="E979" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="980" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A980">
+        <v>979</v>
+      </c>
+      <c r="B980" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C980" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D980">
+        <v>1993</v>
+      </c>
+      <c r="E980" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="981" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A981">
+        <v>980</v>
+      </c>
+      <c r="B981" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C981" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D981">
+        <v>1993</v>
+      </c>
+      <c r="E981" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="982" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A982">
+        <v>981</v>
+      </c>
+      <c r="B982" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C982" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D982">
+        <v>1993</v>
+      </c>
+      <c r="E982" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="983" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A983">
+        <v>982</v>
+      </c>
+      <c r="B983" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C983" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D983">
+        <v>1993</v>
+      </c>
+      <c r="E983" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="984" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A984">
+        <v>983</v>
+      </c>
+      <c r="B984" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C984" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D984">
+        <v>1993</v>
+      </c>
+      <c r="E984" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="985" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A985">
+        <v>984</v>
+      </c>
+      <c r="B985" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C985" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D985">
+        <v>1993</v>
+      </c>
+      <c r="E985" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A986">
+        <v>985</v>
+      </c>
+      <c r="B986" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C986" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D986">
+        <v>1993</v>
+      </c>
+      <c r="E986" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="987" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A987">
+        <v>986</v>
+      </c>
+      <c r="B987" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C987" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D987">
+        <v>1993</v>
+      </c>
+      <c r="E987" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="988" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A988">
+        <v>987</v>
+      </c>
+      <c r="B988" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C988" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D988">
+        <v>1993</v>
+      </c>
+      <c r="E988" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="989" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A989">
+        <v>988</v>
+      </c>
+      <c r="B989" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C989" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D989">
+        <v>1993</v>
+      </c>
+      <c r="E989" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="990" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A990">
+        <v>989</v>
+      </c>
+      <c r="B990" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C990" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D990">
+        <v>1993</v>
+      </c>
+      <c r="E990" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="991" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A991">
+        <v>990</v>
+      </c>
+      <c r="B991" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C991" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D991">
+        <v>1993</v>
+      </c>
+      <c r="E991" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="992" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A992">
+        <v>991</v>
+      </c>
+      <c r="B992" t="s">
+        <v>8</v>
+      </c>
+      <c r="C992" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D992">
+        <v>1993</v>
+      </c>
+      <c r="E992" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="993" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A993">
+        <v>992</v>
+      </c>
+      <c r="B993" t="s">
+        <v>285</v>
+      </c>
+      <c r="C993" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D993">
+        <v>1995</v>
+      </c>
+      <c r="E993" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="994" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A994">
+        <v>993</v>
+      </c>
+      <c r="B994" t="s">
+        <v>286</v>
+      </c>
+      <c r="C994" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D994">
+        <v>1995</v>
+      </c>
+      <c r="E994" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="995" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A995">
+        <v>994</v>
+      </c>
+      <c r="B995" t="s">
+        <v>287</v>
+      </c>
+      <c r="C995" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D995">
+        <v>1995</v>
+      </c>
+      <c r="E995" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="996" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A996">
+        <v>995</v>
+      </c>
+      <c r="B996" t="s">
+        <v>288</v>
+      </c>
+      <c r="C996" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D996">
+        <v>1995</v>
+      </c>
+      <c r="E996" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="997" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A997">
+        <v>996</v>
+      </c>
+      <c r="B997" t="s">
+        <v>289</v>
+      </c>
+      <c r="C997" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D997">
+        <v>1995</v>
+      </c>
+      <c r="E997" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="998" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A998">
+        <v>997</v>
+      </c>
+      <c r="B998" t="s">
+        <v>290</v>
+      </c>
+      <c r="C998" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D998">
+        <v>1995</v>
+      </c>
+      <c r="E998" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="999" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A999">
+        <v>998</v>
+      </c>
+      <c r="B999" t="s">
+        <v>291</v>
+      </c>
+      <c r="C999" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D999">
+        <v>1995</v>
+      </c>
+      <c r="E999" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1000">
+        <v>999</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1000">
+        <v>1995</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1001">
+        <v>1000</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1001">
+        <v>1995</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1002">
+        <v>1001</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1002">
+        <v>1995</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1003">
+        <v>1002</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1003">
+        <v>1995</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1004">
+        <v>1003</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1004">
+        <v>1995</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1005">
+        <v>1004</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>448</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1005">
+        <v>1995</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1006">
+        <v>1005</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1006">
+        <v>1995</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1007">
+        <v>1006</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>449</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1007">
+        <v>1995</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1008">
+        <v>1007</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1008">
+        <v>1995</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1009">
+        <v>1008</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1009">
+        <v>1995</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1010">
+        <v>1009</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1010">
+        <v>1995</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1011">
+        <v>1010</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1011">
+        <v>1995</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1012">
+        <v>1011</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1012">
+        <v>1995</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1013">
+        <v>1012</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1013">
+        <v>1995</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1014">
+        <v>1013</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1014">
+        <v>1995</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1015">
+        <v>1014</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1015">
+        <v>1995</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1016">
+        <v>1015</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1016">
+        <v>1995</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1017">
+        <v>1016</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1017">
+        <v>1995</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1018">
+        <v>1017</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1018">
+        <v>1995</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1019">
+        <v>1018</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1019">
+        <v>1995</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1020">
+        <v>1019</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1020">
+        <v>1995</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1021">
+        <v>1020</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1021">
+        <v>1995</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1022">
+        <v>1021</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1022">
+        <v>1995</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1023">
+        <v>1022</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1023">
+        <v>1995</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1024">
+        <v>1023</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1024">
+        <v>1995</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1025">
+        <v>1024</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1025">
+        <v>1995</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1026">
+        <v>1025</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1026">
+        <v>1995</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1027">
+        <v>1026</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1027">
+        <v>1995</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1028">
+        <v>1027</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1028">
+        <v>1995</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1029">
+        <v>1028</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1029">
+        <v>1995</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1030">
+        <v>1029</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1030">
+        <v>1995</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1031">
+        <v>1030</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1031">
+        <v>1995</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1032">
+        <v>1031</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1032">
+        <v>1995</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1033">
+        <v>1032</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1033">
+        <v>1995</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1034">
+        <v>1033</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1034">
+        <v>1995</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1035">
+        <v>1034</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1035">
+        <v>1995</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>1057</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>